<commit_message>
Etapa 2: se agregó la eliminación de España en la etapa 1 con el comentario y se inició la etapa 2 añadiendo los datos de índice de desarrollo y homicidios, filtrando las top nacionalidades y haciendo un análisis inicial de las variables
</commit_message>
<xml_diff>
--- a/5.1 - Homicidios/homicidios adicionales.xlsx
+++ b/5.1 - Homicidios/homicidios adicionales.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cristian De Andrade\Desktop\Data Science\Tesis Proyecto\Datasets Final - Seleccion\5- World Bank\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cristian De Andrade\Desktop\Data Science\Tesis Proyecto\github\IFM_TMF\5.1 - Homicidios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5AB48B-E53C-419E-B92D-EBA49AF71EDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C31D6153-1A01-4D7E-9A8B-AB34B1353072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33195" yWindow="2925" windowWidth="21600" windowHeight="11385" xr2:uid="{64473E9B-90D3-4E32-B141-FCE053C85C9D}"/>
+    <workbookView xWindow="43200" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{64473E9B-90D3-4E32-B141-FCE053C85C9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,33 +36,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
-  <si>
-    <t>anyo</t>
-  </si>
-  <si>
-    <t>pais</t>
-  </si>
-  <si>
-    <t>Bolivia</t>
-  </si>
-  <si>
-    <t>tasa_homicidios</t>
-  </si>
-  <si>
-    <t>China</t>
-  </si>
-  <si>
-    <t>Senegal</t>
-  </si>
-  <si>
-    <t>Portugal</t>
-  </si>
-  <si>
-    <t>Ukraine</t>
-  </si>
-  <si>
-    <t>Venezuela</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="12">
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Nationality code</t>
+  </si>
+  <si>
+    <t>Homicide Rate</t>
+  </si>
+  <si>
+    <t>BOL</t>
+  </si>
+  <si>
+    <t>CHN</t>
+  </si>
+  <si>
+    <t>SEN</t>
+  </si>
+  <si>
+    <t>PRT</t>
+  </si>
+  <si>
+    <t>VEN</t>
+  </si>
+  <si>
+    <t>UKR</t>
+  </si>
+  <si>
+    <t>CUB</t>
+  </si>
+  <si>
+    <t>PER</t>
+  </si>
+  <si>
+    <t>RUS</t>
   </si>
 </sst>
 </file>
@@ -98,8 +107,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,192 +444,336 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F074647F-FC35-481B-9655-9EC6C5816295}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2008</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>2008</v>
       </c>
       <c r="C2">
         <v>8.52</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
+      <c r="A3">
         <v>2009</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
       </c>
       <c r="C3">
         <v>8.2899999999999991</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
+      <c r="A4">
         <v>2010</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
       </c>
       <c r="C4">
         <v>12.67</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5">
+      <c r="A5">
         <v>2011</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
       </c>
       <c r="C5">
         <v>12.1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6">
+      <c r="A6">
         <v>2012</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
       </c>
       <c r="C6">
         <v>11.77</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7">
+      <c r="A7">
         <v>2013</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
       </c>
       <c r="C7">
         <v>8.84</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8">
+      <c r="A8">
         <v>2014</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
       </c>
       <c r="C8">
         <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B9">
-        <v>2021</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
+      <c r="C9" s="1">
+        <v>0.45</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10">
-        <v>2015</v>
-      </c>
-      <c r="C10">
-        <v>0.27</v>
+      <c r="A10" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.4</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11">
+        <v>2008</v>
+      </c>
+      <c r="B11" t="s">
         <v>6</v>
-      </c>
-      <c r="B11">
-        <v>2008</v>
       </c>
       <c r="C11">
         <v>1.17</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12">
+        <v>2009</v>
+      </c>
+      <c r="B12" t="s">
         <v>6</v>
-      </c>
-      <c r="B12">
-        <v>2009</v>
       </c>
       <c r="C12">
         <v>1.2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13">
+        <v>2022</v>
+      </c>
+      <c r="B13" t="s">
         <v>6</v>
-      </c>
-      <c r="B13">
-        <v>2022</v>
       </c>
       <c r="C13">
         <v>0.72</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14">
+      <c r="A14">
         <v>2013</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
       </c>
       <c r="C14">
         <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15">
+      <c r="A15">
         <v>2018</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
       </c>
       <c r="C15">
         <v>36.69</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16">
+      <c r="A16">
+        <v>2020</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16">
+        <v>4.38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2021</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>2022</v>
       </c>
-      <c r="C16">
-        <v>0</v>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18">
+        <v>4.34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2008</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19">
+        <v>5.27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2009</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20">
+        <v>5.38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2010</v>
+      </c>
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2022</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22">
+        <v>7.08</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2022</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23">
+        <v>7.07</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2011</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24">
+        <v>4.88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2013</v>
+      </c>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <v>5.72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2015</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26">
+        <v>6.16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2016</v>
+      </c>
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>6.16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2022</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28">
+        <v>3.86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2015</v>
+      </c>
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <v>0.27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>